<commit_message>
Cambios de imagenes CN 07 13 CO y REC80
Cambios de imagenes CN 07 13 CO y REC80
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion13/SolicitudGrafica_CN_07_13_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion13/SolicitudGrafica_CN_07_13_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="174">
   <si>
     <t>Fecha:</t>
   </si>
@@ -523,9 +523,6 @@
     <t>http://upload.wikimedia.org/wikipedia/commons/4/47/Schprophase.jpg</t>
   </si>
   <si>
-    <t>http://www.google.com/imgres?imgurl=http://upload.wikimedia.org/wikipedia/commons/c/c7/Sharplan_40C.jpg&amp;imgrefurl=http://en.wikipedia.org/wiki/Laser_scalpel&amp;h=2490&amp;w=1746&amp;tbnid=OSqpBE8hFKfKqM:&amp;zoom=1&amp;docid=F_kqsIpiwMd27M&amp;ei=ZtjrVLuWGOqPsQSlsYKgBw&amp;tbm=isch&amp;ved=0CB4QMygAMAA</t>
-  </si>
-  <si>
     <t>Fotografía de un busto de Hipócrates</t>
   </si>
   <si>
@@ -584,9 +581,6 @@
   </si>
   <si>
     <t>CN_07_13_CO</t>
-  </si>
-  <si>
-    <t>credito:"Sharplan 40C" by Etan J. Tal - Own work. Licensed under CC BY-SA 3.0 via Wikimedia Commons - http://commons.wikimedia.org/wiki/File:Sharplan_40C.jpg#/media/File:Sharplan_40C.jpg</t>
   </si>
   <si>
     <t>dominio publico</t>
@@ -1278,7 +1272,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1335,6 +1329,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1579,6 +1579,12 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="51" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1677,14 +1683,8 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="51" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="59">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1737,6 +1737,12 @@
     <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -2435,7 +2441,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2473,14 +2479,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="98"/>
-      <c r="F2" s="90" t="s">
+      <c r="D2" s="100"/>
+      <c r="F2" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="91"/>
+      <c r="G2" s="93"/>
       <c r="H2" s="48"/>
       <c r="I2" s="48"/>
       <c r="J2" s="16"/>
@@ -2490,14 +2496,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="99">
+      <c r="C3" s="101">
         <v>7</v>
       </c>
-      <c r="D3" s="100"/>
-      <c r="F3" s="92">
+      <c r="D3" s="102"/>
+      <c r="F3" s="94">
         <v>42074</v>
       </c>
-      <c r="G3" s="93"/>
+      <c r="G3" s="95"/>
       <c r="H3" s="48"/>
       <c r="I3" s="48"/>
       <c r="J3" s="16"/>
@@ -2507,10 +2513,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="101" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" s="102"/>
+      <c r="C4" s="103" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="104"/>
       <c r="E4" s="5"/>
       <c r="F4" s="47" t="s">
         <v>55</v>
@@ -2528,10 +2534,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="103" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" s="104"/>
+      <c r="C5" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="106"/>
       <c r="E5" s="5"/>
       <c r="F5" s="45" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2562,7 +2568,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>39</v>
@@ -2580,12 +2586,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="94" t="s">
+      <c r="F8" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="95"/>
-      <c r="H8" s="95"/>
-      <c r="I8" s="96"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="98"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2662,7 +2668,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J10" s="74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="19"/>
     </row>
@@ -2700,10 +2706,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J11" s="81" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K11" s="87" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="12" customFormat="1" ht="57" customHeight="1">
@@ -2740,7 +2746,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J12" s="81" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K12" s="19"/>
     </row>
@@ -2749,7 +2755,7 @@
         <f t="shared" si="0"/>
         <v>IMG04</v>
       </c>
-      <c r="B13" s="124">
+      <c r="B13" s="91">
         <v>152834198</v>
       </c>
       <c r="C13" s="74" t="s">
@@ -2778,7 +2784,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="82" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K13" s="89"/>
     </row>
@@ -2816,10 +2822,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="81" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K14" s="87" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="75" customHeight="1">
@@ -2834,7 +2840,7 @@
         <v>145</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E15" s="74" t="s">
         <v>147</v>
@@ -2856,10 +2862,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="K15" s="123" t="s">
-        <v>175</v>
+        <v>156</v>
+      </c>
+      <c r="K15" s="90" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="23" customHeight="1">
@@ -2896,7 +2902,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="83" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K16" s="29"/>
     </row>
@@ -2934,7 +2940,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="84" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K17" s="21"/>
     </row>
@@ -2972,17 +2978,17 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J18" s="84" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="72">
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="14">
       <c r="A19" s="13" t="str">
         <f t="shared" si="0"/>
         <v>IMG10</v>
       </c>
-      <c r="B19" s="78" t="s">
-        <v>151</v>
+      <c r="B19" s="78">
+        <v>144666932</v>
       </c>
       <c r="C19" s="74" t="s">
         <v>145</v>
@@ -3010,11 +3016,9 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="86" t="s">
-        <v>161</v>
-      </c>
-      <c r="K19" s="88" t="s">
-        <v>172</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="K19" s="88"/>
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" ht="57" customHeight="1">
       <c r="A20" s="13" t="str">
@@ -3050,7 +3054,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J20" s="81" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K20" s="21"/>
     </row>
@@ -3088,7 +3092,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J21" s="84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K21" s="21"/>
     </row>
@@ -3126,7 +3130,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J22" s="85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K22" s="20"/>
     </row>
@@ -3164,7 +3168,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J23" s="81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K23" s="19"/>
     </row>
@@ -3202,7 +3206,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J24" s="74" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K24" s="15"/>
     </row>
@@ -3240,7 +3244,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="74" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K25" s="19"/>
     </row>
@@ -3278,7 +3282,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J26" s="74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K26" s="19"/>
     </row>
@@ -5912,25 +5916,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" thickBot="1">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="109"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="111"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="38" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="39"/>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="111"/>
-      <c r="E2" s="112"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="114"/>
       <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:11" ht="60">
@@ -5938,11 +5942,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="116" t="s">
+      <c r="C3" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="117"/>
-      <c r="E3" s="118"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="120"/>
       <c r="F3" s="40"/>
       <c r="H3" s="30" t="s">
         <v>18</v>
@@ -5993,11 +5997,11 @@
       <c r="C5" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="119" t="str">
+      <c r="D5" s="121" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="120"/>
+      <c r="E5" s="122"/>
       <c r="F5" s="40"/>
       <c r="H5" s="30" t="s">
         <v>22</v>
@@ -6042,12 +6046,12 @@
       <c r="C7" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="105" t="str">
+      <c r="D7" s="107" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="105"/>
-      <c r="F7" s="106"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="108"/>
       <c r="H7" s="30" t="s">
         <v>24</v>
       </c>
@@ -6141,14 +6145,14 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="107" t="s">
+      <c r="A13" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="108"/>
-      <c r="C13" s="108"/>
-      <c r="D13" s="108"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="109"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="111"/>
       <c r="I13" s="30" t="s">
         <v>33</v>
       </c>
@@ -6181,12 +6185,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="39"/>
-      <c r="C15" s="110" t="s">
+      <c r="C15" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="111"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="112"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="114"/>
       <c r="J15" s="30">
         <v>12</v>
       </c>
@@ -6226,12 +6230,12 @@
       <c r="C17" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="113" t="str">
+      <c r="D17" s="115" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="114"/>
-      <c r="F17" s="115"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="117"/>
       <c r="J17" s="30">
         <v>14</v>
       </c>
@@ -6247,12 +6251,12 @@
       <c r="C18" s="70" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="105" t="str">
+      <c r="D18" s="107" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="105"/>
-      <c r="F18" s="106"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="108"/>
       <c r="J18" s="30">
         <v>15</v>
       </c>
@@ -6657,41 +6661,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="123" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="121" t="s">
+      <c r="C1" s="123" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="121" t="s">
+      <c r="D1" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="121" t="s">
+      <c r="E1" s="123" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="121" t="s">
+      <c r="F1" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="121" t="s">
+      <c r="G1" s="123" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="122" t="s">
+      <c r="H1" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="121"/>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
+      <c r="A2" s="123"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
       <c r="H2" s="49" t="s">
         <v>65</v>
       </c>

</xml_diff>